<commit_message>
pawan changes added :paysafe
</commit_message>
<xml_diff>
--- a/src/conf/ChargeBackMetadata.xlsx
+++ b/src/conf/ChargeBackMetadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14655" windowHeight="6000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14655" windowHeight="6000"/>
   </bookViews>
   <sheets>
     <sheet name="Paysafe" sheetId="2" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>com.ibaseit.scraping.handler.HtmlHandler</t>
   </si>
   <si>
-    <t>com.ibaseit.scraping.handler.ExcelHandler</t>
-  </si>
-  <si>
     <t>42162</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>?__EVENTVALIDATION</t>
+  </si>
+  <si>
+    <t>com.ibaseit.scraping.handler.PaysafeHandler</t>
   </si>
 </sst>
 </file>
@@ -691,18 +691,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.25" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -816,7 +816,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>41</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>42</v>
@@ -886,21 +886,21 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="1"/>
     </row>
@@ -909,7 +909,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -917,100 +917,100 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" s="1"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42" s="1"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B43" s="1"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>43</v>
@@ -1018,34 +1018,34 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>16</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1071,14 +1071,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="136.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1166,7 +1166,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1236,7 +1236,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="1"/>
     </row>
@@ -1302,7 +1302,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
         <v>27</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,7 +1346,7 @@
         <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1354,7 +1354,7 @@
         <v>31</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
         <v>32</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1414,7 +1414,7 @@
         <v>16</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1437,11 +1437,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1486,10 +1486,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
@@ -1553,10 +1553,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
@@ -1581,7 +1581,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
VIMAS : Hari  humboldt : pawan vps aurora and mongodb : dinesh changes added
</commit_message>
<xml_diff>
--- a/src/conf/ChargeBackMetadata.xlsx
+++ b/src/conf/ChargeBackMetadata.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14655" windowHeight="6000"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14655" windowHeight="6000" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Paysafe" sheetId="2" r:id="rId1"/>
-    <sheet name="VIMAS" sheetId="3" r:id="rId2"/>
-    <sheet name="ClientDetails" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="ClientDetails" sheetId="4" r:id="rId1"/>
+    <sheet name="Paysafe" sheetId="2" r:id="rId2"/>
+    <sheet name="VIMAS" sheetId="3" r:id="rId3"/>
+    <sheet name="VPSAurora" sheetId="6" r:id="rId4"/>
+    <sheet name="HumboldtNMA" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="133">
   <si>
     <t>https://merituspayment.com/merchants/frmLogin.aspx</t>
   </si>
@@ -293,13 +294,136 @@
   </si>
   <si>
     <t>com.ibaseit.scraping.handler.PaysafeHandler</t>
+  </si>
+  <si>
+    <t>Step5</t>
+  </si>
+  <si>
+    <t>Charge Back Record Details</t>
+  </si>
+  <si>
+    <t>https://vimas.cynergydata.com/Vimas2.0/Merchant/Report_Chargebacks_Record.aspx?CaseNum=$1&amp;Intmid=$2</t>
+  </si>
+  <si>
+    <t>com.ibaseit.scraping.handler.VimasRecordHandler</t>
+  </si>
+  <si>
+    <t>https://aurora.visionpayments.com/aurora2/login.php</t>
+  </si>
+  <si>
+    <t>auth_username</t>
+  </si>
+  <si>
+    <t>auth_password</t>
+  </si>
+  <si>
+    <t>ChargeBack cases Get</t>
+  </si>
+  <si>
+    <t>https://aurora.visionpayments.com/aurora2/merchant/tab_sub_m_chargeback.php?aurora_id=32634&amp;selected_tab=s1&amp;base_referer=tabs.php</t>
+  </si>
+  <si>
+    <t>com.ibaseit.scraping.handler.AuroraHandler</t>
+  </si>
+  <si>
+    <t>VPSAurora</t>
+  </si>
+  <si>
+    <t>27260019549401</t>
+  </si>
+  <si>
+    <t>C0mcastic!</t>
+  </si>
+  <si>
+    <t>HumboldtNMA</t>
+  </si>
+  <si>
+    <t>cl.mccurdc10</t>
+  </si>
+  <si>
+    <t>25Oct2016</t>
+  </si>
+  <si>
+    <t>Humboldt/NMA</t>
+  </si>
+  <si>
+    <t>https://www.myclientline.net/ssofiles/login.html</t>
+  </si>
+  <si>
+    <t>https://www.myclientline.net/portal/portal/siteminderagent/forms/login.fcc</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>Navigate next page</t>
+  </si>
+  <si>
+    <t>https://www.myclientline.net/portalJ/clrchandler2J/CLRNET/login.aspx</t>
+  </si>
+  <si>
+    <t>tamtkn</t>
+  </si>
+  <si>
+    <t>000270923D676EEC279D0F80</t>
+  </si>
+  <si>
+    <t>CISP_COMPLIANCE</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>DDA_COMPLIANCE</t>
+  </si>
+  <si>
+    <t>https://www.myclientline.net/clrnet/Disputes/Chargeback.aspx?strRqstID=897208966886&amp;intRqstLevel=120&amp;strStartDate=10%2f13%2f2016&amp;strEndDate=11%2f01%2f2016&amp;strSelectDateType=R&amp;dblStartAmount=-999999999&amp;dblEndAmount=999999999&amp;strChStatus=ALL&amp;strCat=0&amp;strCardOrRefNumber=&amp;strCardOrRefType=C&amp;strRecordType=A&amp;strReasonCode=0</t>
+  </si>
+  <si>
+    <t>ctl00_Content_ToolkitScriptManager1_HiddenField</t>
+  </si>
+  <si>
+    <t>/wEPDwULLTExMjA2OTAxMTkPZBYCZg9kFgICAQ9kFggCAw8PFgIeCEltYWdlVXJsBRt+L0ltYWdlcy9sb2dvcy9GRENfbG9nby5qcGdkZAIFDxBkZBYBZmQCCQ88KwANAgAPFgIeC18hRGF0YUJvdW5kZ2QMFCsACgUjMDowLDA6MSwwOjIsMDozLDA6NCwwOjUsMDo2LDA6NywwOjgUKwACFgYeBFRleHQFCURhc2hib2FyZB4LTmF2aWdhdGVVcmxlHgpTZWxlY3RhYmxlaBQrAAQFCzA6MCwwOjEsMDoyFCsAAhYEHwIFE1JlcG9ydGluZyBEYXNoYm9hcmQfAwUgL2Nscm5ldC9EYXNoYm9hcmQvUmVwb3J0aW5nLmFzcHhkFCsAAhYEHwIFEkRpc3B1dGVzIERhc2hib2FyZB8DBR8vY2xybmV0L0Rhc2hib2FyZC9EaXNwdXRlcy5hc3B4ZBQrAAIWBB8CBQxUb2RheSdzIERhdGEfAwUhL2Nscm5ldC9EYXNoYm9hcmQvVG9kYXlzRGF0YS5hc3B4ZBQrAAIWBh8CBQVTYWxlcx8DZR8EaBQrAAkFHzA6MCwwOjEsMDoyLDA6MywwOjQsMDo1LDA6NiwwOjcUKwACFgQfAgUTQ3JlZGl0IFRyYW5zYWN0aW9ucx8DBRkvY2xybmV0L1NhbGVzL0NyZWRpdC5hc3B4ZBQrAAIWBB8CBRJEZWJpdCBUcmFuc2FjdGlvbnMfAwUYL2Nscm5ldC9TYWxlcy9EZWJpdC5hc3B4ZBQrAAIWBB8CBQxDaGVjayBEcmFmdHMfAwUdL2Nscm5ldC9TYWxlcy9DaGVja0RyYWZ0LmFzcHhkFCsAAhYEHwIFF0NoZWNrIFBhcGVyL0VsZWN0cm9uaWNzHwMFHS9jbHJuZXQvU2FsZXMvQ2hlY2tQYXBlci5hc3B4ZBQrAAIWBB8CBRVUZXJtaW5hbCBUcmFuc2FjdGlvbnMfAwUbL2Nscm5ldC9TYWxlcy9UZXJtaW5hbC5hc3B4ZBQrAAIWBB8CBRVSZWplY3RlZCBUcmFuc2FjdGlvbnMfAwUaL2Nscm5ldC9TYWxlcy9SZWplY3RzLmFzcHhkFCsAAhYEHwIFE1RyYW5zYWN0aW9uIFN1bW1hcnkfAwUlL2Nscm5ldC9TYWxlcy9UcmFuc2FjdGlvblN1bW1hcnkuYXNweGQUKwACFgQfAgUVTW9udGhseSBTYWxlcyBIaXN0b3J5HwMFHy9jbHJuZXQvU2FsZXMvTW9udGhseVNhbGVzLmFzcHhkFCsAAhYGHwIFB0Z1bmRpbmcfA2UfBGgUKwAGBRMwOjAsMDoxLDA6MiwwOjMsMDo0FCsAAhYEHwIFDUJhbmsgRGVwb3NpdHMfAwUhL2Nscm5ldC9GdW5kaW5nL0JhbmtEZXBvc2l0cy5hc3B4ZBQrAAIWBB8CBRRBbGwgQWN0aXZpdHkgU3VtbWFyeR8DBScvY2xybmV0L0Z1bmRpbmcvQWxsQWN0aXZpdHlTdW1tYXJ5LmFzcHhkFCsAAhYEHwIFDldpdGhIZWxkIEZ1bmRzHwMFIi9jbHJuZXQvRnVuZGluZy9XaXRoaGVsZEZ1bmRzLmFzcHhkFCsAAhYEHwIFJk1vbnRobHkgRmVlIGFuZCBTZXJ2aWNlIENoYXJnZSBIaXN0b3J5HwMFHy9jbHJuZXQvRnVuZGluZy9Nb250aGx5RmVlLmFzcHhkFCsAAhYEHwIFEU1vbnRobHkgU3RhdGVtZW50HwMFJS9jbHJuZXQvRnVuZGluZy9Nb250aGx5U3RhdGVtZW50LmFzcHhkFCsAAhYGHwIFDVJhdGUgQW5hbHlzaXMfA2UfBGgUKwAEBQswOjAsMDoxLDA6MhQrAAIWBB8CBRZRdWFsaWZpY2F0aW9uIEFuYWx5c2lzHwMFMC9jbHJuZXQvUmF0ZSBBbmFseXNpcy9RdWFsaWZpY2F0aW9uQW5hbHlzaXMuYXNweGQUKwACFgQfAgUVUXVhbGlmaWNhdGlvbiBFeHBlbnNlHwMFLy9jbHJuZXQvUmF0ZSBBbmFseXNpcy9RdWFsaWZpY2F0aW9uRXhwZW5zZS5hc3B4ZBQrAAIWBB8CBQlCaWxsYmFja3MfAwUkL2Nscm5ldC9SYXRlIEFuYWx5c2lzL0JpbGxiYWNrcy5hc3B4ZBQrAAIWBh8CBQhEaXNwdXRlcx8DZR8EaBQrAAYFEzA6MCwwOjEsMDoyLDA6MywwOjQUKwACFgQfAgULQ2hhcmdlYmFja3MfAwUgL2Nscm5ldC9EaXNwdXRlcy9DaGFyZ2ViYWNrLmFzcHhkFCsAAhYEHwIFClJldHJpZXZhbHMfAwUgL2Nscm5ldC9EaXNwdXRlcy9SZXRyaWV2YWxzLmFzcHhkFCsAAhYEHwIFE0NoYXJnZWJhY2sgQW5hbHlzaXMfAwUoL2Nscm5ldC9EaXNwdXRlcy9DaGFyZ2VCYWNrQW5hbHlzaXMuYXNweGQUKwACFgQfAgUSUmV0cmlldmFsIEFuYWx5c2lzHwMFJy9jbHJuZXQvRGlzcHV0ZXMvUmV0cmlldmFsQW5hbHlzaXMuYXNweGQUKwACFgQfAgUORXhjZXNzaXZlIFJpc2sfAwUqL2Nscm5ldC9EaXNwdXRlcy9FeGNlc3NpdmVSaXNrU3VtbWFyeS5hc3B4ZBQrAAIWBh8CBQhSZXNlYXJjaB8DZR8EaBQrAAkFHzA6MCwwOjEsMDoyLDA6MywwOjQsMDo1LDA6NiwwOjcUKwACFgQfAgULQ2FyZCBTZWFyY2gfAwUgL2Nscm5ldC9SZXNlYXJjaC9DYXJkU2VhcmNoLmFzcHhkFCsAAhYEHwIFFEF1dGhvcml6YXRpb24gU2VhcmNoHwMFKS9jbHJuZXQvUmVzZWFyY2gvQXV0aG9yaXphdGlvblNlYXJjaC5hc3B4ZBQrAAIWBB8CBQ1RdWVyeSBCdWlsZGVyHwMFIi9jbHJuZXQvUmVzZWFyY2gvUXVlcnlCdWlsZGVyLmFzcHhkFCsAAhYEHwIFGExvY2F0aW9uIFByb2ZpbGUgRGV0YWlscx8DBSUvY2xybmV0L1Jlc2VhcmNoL0xvY2F0aW9uUHJvZmlsZS5hc3B4ZBQrAAIWBB8CBRpDYXJkIElzc3VlciBJZGVudGlmaWNhdGlvbh8DBSAvY2xybmV0L1Jlc2VhcmNoL0NhcmRJc3N1ZXIuYXNweGQUKwACFgQfAgUTQ2hlY2sgQXV0aG9yaXphdGlvbh8DBR8vY2xybmV0L1Jlc2VhcmNoL0NoZWNrQXV0aC5hc3B4ZBQrAAIWBB8CBQ9GcmF1ZCBSZXBvcnRpbmcfAwUkL2Nscm5ldC9SZXNlYXJjaC9GcmF1ZFJlcG9ydGluZy5hc3B4ZBQrAAIWBB8CBRRSZWZ1bmQgV2l0aCBObyBTYWxlcx8DBSMvY2xybmV0L1Jlc2VhcmNoL1JlZnVuZHNOb1NhbGUuYXNweGQUKwACFgYfAgUHUmVwb3J0cx8DZR8EaBQrAAUFDzA6MCwwOjEsMDoyLDA6MxQrAAIWBB8CBRBTY2hlZHVsZSBSZXBvcnRzHwMFJC9jbHJuZXQvUmVwb3J0cy9TY2hlZHVsZVJlcG9ydHMuYXNweGQUKwACFgQfAgUMVmlldyBSZXBvcnRzHwMFIC9jbHJuZXQvUmVwb3J0cy9WaWV3UmVwb3J0cy5hc3B4ZBQrAAIWBB8CBQ5VcGRhdGUgUmVwb3J0cx8DBSIvY2xybmV0L1JlcG9ydHMvVXBkYXRlUmVwb3J0cy5hc3B4ZBQrAAIWBB8CBQ5EZWxldGUgUmVwb3J0cx8DBSIvY2xybmV0L1JlcG9ydHMvRGVsZXRlUmVwb3J0cy5hc3B4ZBQrAAIWBh8CBQlHaWZ0Y2FyZHMfA2UfBGgUKwACBQMwOjAUKwACFgQfAgUJR2lmdGNhcmRzHwMFIC9jbHJuZXQvR2lmdGNhcmRzL0dpZnRDYXJkcy5hc3B4ZBQrAAIWBh8CBQlSZWZlcmVuY2UfA2UfBGgUKwAEBQswOjAsMDoxLDA6MhQrAAIWBB8CBQREZW1vHwMFGi9jbHJuZXQvUmVmZXJlbmNlL0RlbW8uYXNwZBQrAAIWBB8CBQhUdXRvcmlhbB8DBR4vY2xybmV0L1JlZmVyZW5jZS9UdXRvcmlhbC5hc3BkFCsAAhYEHwIFClVzZXIgZ3VpZGUfAwUfL2Nscm5ldC9SZWZlcmVuY2UvVXNlckd1aWRlLmFzcGRkAgsPZBYGAgcPFgIfAgUPQ2hhcmdlYmFjayBMaXN0ZAIJDw8WAh4HVmlzaWJsZWhkFgoCAQ9kFgoCAw8PFgIfAmVkZAIFDw8WAh8FZxYCHgdvbmNsaWNrBfcCdmFyIHNldFNpemUgPSAnZGlhbG9nSGVpZ2h0OjYwMHB4O2RpYWxvZ1dpZHRoOjYwMHB4O2NlbnRlcjp5ZXM7c2Nyb2xsYmFyczp5ZXM7cmVzaXphYmxlOm5vO3Rvb2xiYXI6bm87c3RhdHVzOm5vO21lbnViYXI6bm8nO3ZhciByZXR1cm5EYXRhPXdpbmRvdy5zaG93TW9kYWxEaWFsb2coJy4uL0Z1bmRpbmcvTWVyY2hhbnREREFMb29rdXAuYXNweD9zdHJTZWFyY2hUeXBlPU0nLCd0ZW1wJyxzZXRTaXplKTtpZihyZXR1cm5EYXRhPT11bmRlZmluZWQpe3JldHVybkRhdGE9Jyc7fWVsc2V7ZG9jdW1lbnQuZ2V0RWxlbWVudEJ5SWQoImN0bDAwX0NvbnRlbnRfQ3RsSGllcmFjaHkxX3R4dE1lcmNoYW50SWQiKS52YWx1ZT1yZXR1cm5EYXRhO31yZXR1cm4gZmFsc2U7ZAIHDxBkZBYAZAIJDxAPFgIfBWhkEBUCBFNZU1AEU1lTUxUCBFNZU1AEU1lTUxQrAwJnZxYBZmQCCw8PFgIfBWhkZAIOD2QWAmYPZBYCAgEPEGRkFgFmZAIQD2QWAmYPZBYCAgEPEGRkFgFmZAISDxBkZBYAZAIUD2QWAmYPZBYCAgMPEGRkFgFmZAILD2QWGgIBD2QWBAIBDw8WAh8CBS5Mb2NhdGlvbiAtIDg5NzIwODk2Njg4NiAtIE1BUlZFTE9VUyBTS0lOIFNFUlVNZGQCAw8PFgIfAgUrU3RhdHVzIERhdGUgUmFuZ2U6IDEwLzEzLzIwMTYgdG8gMTEvMDEvMjAxNmRkAgcPDxYCHwIFFFJlY29yZCAxIHRvIDEwIG9mIDEwZGQCCQ8PFgIfAgULUGFnZSAxIG9mIDFkZAILDw8WAh4HRW5hYmxlZGhkZAINDw8WAh8HaGRkAg8PDxYCHwdoZGQCEQ8PFgIfB2hkZAIVDxBkEBUBATEVAQExFCsDAWcWAWZkAhcPDxYCHwVoZGQCGQ8PFgIfBWhkZAIbDw8WAh8FaGRkAh0PDxYCHwVoZGQCHw8PFgIfBWhkZBgCBR5fX0NvbnRyb2xzUmVxdWlyZVBvc3RCYWNrS2V5X18WAgUpY3RsMDAkQ29udGVudCRFeHBvcnRCdXR0b24kaW1nRXhwb3J0RXhjZWwFJ2N0bDAwJENvbnRlbnQkRXhwb3J0QnV0dG9uJGltZ0V4cG9ydENTVgUbY3RsMDAkQ29udGVudCRndkNoYXJnZWJhY2tzDzwrAAwBCAIBZCksBkfpyFz5oyuNicoSxGww8v4OM25x9H8WPQTP1FFs</t>
+  </si>
+  <si>
+    <t>1A19D298</t>
+  </si>
+  <si>
+    <t>ctl00$Language</t>
+  </si>
+  <si>
+    <t>EN-US</t>
+  </si>
+  <si>
+    <t>ctl00$Content$txtPageNum</t>
+  </si>
+  <si>
+    <t>ctl00$Content$txtLocNum</t>
+  </si>
+  <si>
+    <t>ctl00$Content$ExportButton$imgExportExcel.x</t>
+  </si>
+  <si>
+    <t>ctl00$Content$ExportButton$imgExportExcel.y</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>ctl00$Content$ddlPageSelector</t>
+  </si>
+  <si>
+    <t>com.ibaseit.scraping.handler.HumboldtNMAHandler</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,13 +459,44 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF545454"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -372,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -387,6 +542,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -689,20 +851,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.25" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1067,18 +1337,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="136.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1417,222 +1687,644 @@
         <v>87</v>
       </c>
     </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B33" r:id="rId1"/>
     <hyperlink ref="B23" r:id="rId2"/>
+    <hyperlink ref="B52" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="200" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="200" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="131.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1"/>
+      <c r="A17" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="1"/>
+      <c r="A18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>41</v>
+      <c r="A19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46" s="11"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1"/>
+    <hyperlink ref="B34" display="https://www.myclientline.net/clrnet/Disputes/Chargeback.aspx?strRqstID=897208966886&amp;intRqstLevel=120&amp;strStartDate=10%2f13%2f2016&amp;strEndDate=11%2f01%2f2016&amp;strSelectDateType=R&amp;dblStartAmount=-999999999&amp;dblEndAmount=999999999&amp;strChStatus=ALL&amp;strCat=0&amp;strCar"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>